<commit_message>
Update blueprints, choreography BPMN, Oral Presentation slides
</commit_message>
<xml_diff>
--- a/Blueprints/BlueprintAssociations.xlsx
+++ b/Blueprints/BlueprintAssociations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaur\Documents\UTC\3- Semestre P19 - GI04 - Erasmus\Courses\Process &amp; Service Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaur\Documents\UTC\3- Semestre P19 - GI04 - Erasmus\Courses\Process &amp; Service Design\Project\Blueprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13FE76D-9C40-403A-86AF-4ACDC4C96C7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16720C18-D7AE-4A2E-AEC3-061C61A5FF87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>AWARE</t>
   </si>
@@ -102,15 +102,6 @@
     <t>Link to the website, QR Code for the app</t>
   </si>
   <si>
-    <t>Homepage of the website with information on the association</t>
-  </si>
-  <si>
-    <t>Presentation of the association</t>
-  </si>
-  <si>
-    <t>Presentation of the association, link to the website</t>
-  </si>
-  <si>
     <t>Downloads the app</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>Requests for food</t>
   </si>
   <si>
-    <t>Inserts the adress and select a type of company</t>
-  </si>
-  <si>
     <t>Amazon Simple Notification Service</t>
   </si>
   <si>
@@ -150,18 +138,9 @@
     <t>Database: creation of a new request</t>
   </si>
   <si>
-    <t>Inserts the adress and select a type of food company</t>
-  </si>
-  <si>
     <t>Fills form about reasons of the departure</t>
   </si>
   <si>
-    <t>Database: insertion of a new reason of departure</t>
-  </si>
-  <si>
-    <t>Checks one reason of departure in a list</t>
-  </si>
-  <si>
     <t>Deletes account</t>
   </si>
   <si>
@@ -193,6 +172,21 @@
   </si>
   <si>
     <t>SERVICE NAME: DONOTHROW</t>
+  </si>
+  <si>
+    <t>Checks some reasons of departure in a list</t>
+  </si>
+  <si>
+    <t>Inserts address and type of food needed</t>
+  </si>
+  <si>
+    <t>Homepage of the website with information on Donothrow</t>
+  </si>
+  <si>
+    <t>Presentation of Donothrow, link to the website</t>
+  </si>
+  <si>
+    <t>Presentation of Donothrow</t>
   </si>
 </sst>
 </file>
@@ -994,7 +988,7 @@
   <dimension ref="B1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1008,7 +1002,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="49.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="36" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -1056,31 +1050,31 @@
         <v>22</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>35</v>
-      </c>
       <c r="K5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1110,7 +1104,7 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="19" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -1143,46 +1137,46 @@
       <c r="N8" s="21"/>
       <c r="O8" s="31"/>
     </row>
-    <row r="9" spans="2:15" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="40"/>
       <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>33</v>
-      </c>
       <c r="J9" s="21" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O9" s="31"/>
     </row>
     <row r="10" spans="2:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="40"/>
       <c r="C10" s="13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="21"/>
@@ -1196,7 +1190,7 @@
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
       <c r="O10" s="31" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1207,29 +1201,29 @@
       <c r="D11" s="20"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="21" t="s">
-        <v>33</v>
-      </c>
       <c r="J11" s="21" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="K11" s="21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O11" s="31"/>
     </row>
@@ -1281,23 +1275,21 @@
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="25" t="s">
-        <v>34</v>
-      </c>
       <c r="J14" s="25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="M14" s="25" t="s">
-        <v>42</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="M14" s="25"/>
       <c r="N14" s="25" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="O14" s="33"/>
     </row>
@@ -1312,13 +1304,13 @@
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>

</xml_diff>

<commit_message>
add blueprint for individuals to presentation slides
</commit_message>
<xml_diff>
--- a/Blueprints/BlueprintAssociations.xlsx
+++ b/Blueprints/BlueprintAssociations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaur\Documents\UTC\3- Semestre P19 - GI04 - Erasmus\Courses\Process &amp; Service Design\Project\Blueprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaur\Documents\UTC\3- Semestre P19 - GI04 - Erasmus\Courses\Process &amp; Service Design\process_and_service\Blueprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16720C18-D7AE-4A2E-AEC3-061C61A5FF87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310AA0E-40A6-4B06-9E89-9428DA0604A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>AWARE</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Step</t>
   </si>
   <si>
-    <t>Experience</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -61,12 +58,6 @@
   </si>
   <si>
     <t>Mobile</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Customer service</t>
   </si>
   <si>
     <t>IT-Department</t>
@@ -249,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -462,21 +453,6 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -511,17 +487,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -564,6 +529,84 @@
         <color auto="1"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -572,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,15 +630,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,89 +642,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -702,7 +724,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -985,344 +1013,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O33"/>
+  <dimension ref="B1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20.296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="17.09765625" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
     <col min="6" max="6" width="15.09765625" customWidth="1"/>
-    <col min="7" max="15" width="13" customWidth="1"/>
+    <col min="7" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
+    <col min="12" max="12" width="18.09765625" customWidth="1"/>
+    <col min="13" max="13" width="18.3984375" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="49.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
-        <v>47</v>
+      <c r="B1" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:15" s="2" customFormat="1" ht="52.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43" t="s">
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43" t="s">
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
     </row>
-    <row r="5" spans="2:15" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="45" t="s">
+    <row r="5" spans="2:15" ht="62.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="19"/>
+    </row>
+    <row r="7" spans="2:15" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="39"/>
+      <c r="C7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="2:15" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="39"/>
+      <c r="C8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="2:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="39"/>
+      <c r="C9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="111.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="40"/>
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="32"/>
+    </row>
+    <row r="11" spans="2:15" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="29"/>
+    </row>
+    <row r="12" spans="2:15" ht="62.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="34"/>
+      <c r="C12" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>38</v>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="41"/>
-      <c r="C6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="29"/>
+    <row r="13" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
     </row>
-    <row r="7" spans="2:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="30"/>
-    </row>
-    <row r="8" spans="2:15" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="40"/>
-      <c r="C8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="31"/>
-    </row>
-    <row r="9" spans="2:15" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
-      <c r="C9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" s="31"/>
-    </row>
-    <row r="10" spans="2:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="40"/>
-      <c r="C10" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
-      <c r="C11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" s="31"/>
-    </row>
-    <row r="12" spans="2:15" ht="52.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="41"/>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="38"/>
-    </row>
-    <row r="13" spans="2:15" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="32"/>
-    </row>
-    <row r="14" spans="2:15" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="C14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="O14" s="33"/>
-    </row>
-    <row r="15" spans="2:15" ht="62.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="41"/>
-      <c r="C15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="9"/>
-    </row>
+    <row r="14" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1337,18 +1318,14 @@
     <row r="28" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="30" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B13:B15"/>
+  <mergeCells count="6">
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="M4:O4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B6:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>